<commit_message>
Atualização Tabela Níveis Críticos
</commit_message>
<xml_diff>
--- a/Tabelas níveis críticos.xlsx
+++ b/Tabelas níveis críticos.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25803"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9DA3A626-56BA-4294-B782-916726C8C44B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Samuel\Documents\Arquivos SP Tech\Arquitetura Computacional\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE8E0E8C-7D8E-41AB-97B8-61486388758A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="15">
   <si>
     <t>Temperatura</t>
   </si>
@@ -49,13 +49,40 @@
   </si>
   <si>
     <t>Umidade</t>
+  </si>
+  <si>
+    <t>35.0°</t>
+  </si>
+  <si>
+    <t>33.0°</t>
+  </si>
+  <si>
+    <t>31.0°</t>
+  </si>
+  <si>
+    <t>30.0°</t>
+  </si>
+  <si>
+    <t>25.0°</t>
+  </si>
+  <si>
+    <t>23.0°</t>
+  </si>
+  <si>
+    <t>20.0°</t>
+  </si>
+  <si>
+    <t>18.0°</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -83,7 +110,16 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
+      <b/>
+      <sz val="14"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -91,21 +127,22 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -164,7 +201,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -204,14 +241,27 @@
     </border>
     <border>
       <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
       <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -220,9 +270,7 @@
         <color rgb="FF3F3F3F"/>
       </left>
       <right/>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -231,9 +279,7 @@
       <right style="thin">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -247,21 +293,6 @@
   </cellStyleXfs>
   <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -277,25 +308,40 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="9" fontId="5" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="6" fillId="8" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="5" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="5" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="2" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="9" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
-    <cellStyle name="Accent2" xfId="3" builtinId="33"/>
-    <cellStyle name="Accent4" xfId="4" builtinId="41"/>
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
+    <cellStyle name="Ênfase2" xfId="3" builtinId="33"/>
+    <cellStyle name="Ênfase4" xfId="4" builtinId="41"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Output" xfId="2" builtinId="21"/>
+    <cellStyle name="Ruim" xfId="1" builtinId="27"/>
+    <cellStyle name="Saída" xfId="2" builtinId="21"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
@@ -311,7 +357,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -609,140 +655,140 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="8" width="13.7109375" style="1" customWidth="1"/>
+    <col min="1" max="8" width="16.7109375" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2"/>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
     </row>
-    <row r="2" spans="1:8">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="5"/>
-      <c r="F2" s="3" t="s">
+      <c r="E2" s="10"/>
+      <c r="F2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:8">
-      <c r="A3" s="6">
-        <v>0</v>
-      </c>
-      <c r="B3" s="7">
-        <v>0</v>
-      </c>
-      <c r="C3" s="8">
-        <v>0</v>
-      </c>
-      <c r="D3" s="9">
-        <v>0</v>
-      </c>
-      <c r="E3" s="9">
-        <v>0</v>
-      </c>
-      <c r="F3" s="8">
-        <v>0</v>
-      </c>
-      <c r="G3" s="7">
-        <v>0</v>
-      </c>
-      <c r="H3" s="6">
-        <v>0</v>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:8">
-      <c r="A4" s="10"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" s="5"/>
     </row>
-    <row r="5" spans="1:8" ht="15.75">
-      <c r="A5" s="2" t="s">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
+      <c r="B5" s="8"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
     </row>
-    <row r="6" spans="1:8">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="5"/>
-      <c r="F6" s="3" t="s">
+      <c r="E6" s="10"/>
+      <c r="F6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="G6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="H6" s="3" t="s">
+      <c r="H6" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="11">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="B7" s="12">
-        <v>0</v>
+        <v>0.08</v>
       </c>
       <c r="C7" s="13">
-        <v>0</v>
+        <v>0.09</v>
       </c>
       <c r="D7" s="14">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="E7" s="14">
-        <v>0</v>
+        <v>0.12</v>
       </c>
       <c r="F7" s="13">
-        <v>0</v>
+        <v>0.13</v>
       </c>
       <c r="G7" s="12">
-        <v>0</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="H7" s="11">
-        <v>0</v>
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -753,5 +799,6 @@
     <mergeCell ref="D6:E6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="5" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>